<commit_message>
working on adding comments
</commit_message>
<xml_diff>
--- a/output/ROC Curve Test Data_Made Up (1)_z100.0_results.xlsx
+++ b/output/ROC Curve Test Data_Made Up (1)_z100.0_results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="83">
   <si>
     <t>Channel G</t>
   </si>
@@ -224,16 +224,16 @@
     <t>F True Negative</t>
   </si>
   <si>
-    <t>False Positive Rate (Channel G)</t>
-  </si>
-  <si>
-    <t>True Positive Rate (Channel G)</t>
-  </si>
-  <si>
-    <t>False Positive Rate (Channel F)</t>
-  </si>
-  <si>
-    <t>True Positive Rate (Channel F)</t>
+    <t>FPR (G)</t>
+  </si>
+  <si>
+    <t>TPR (G)</t>
+  </si>
+  <si>
+    <t>FPR (F)</t>
+  </si>
+  <si>
+    <t>TPR (F)</t>
   </si>
   <si>
     <t>FPR (Combined)</t>
@@ -242,22 +242,28 @@
     <t>TPR (Combined)</t>
   </si>
   <si>
-    <t>Confusion Matrix</t>
-  </si>
-  <si>
     <t>Channel</t>
   </si>
   <si>
-    <t>False Positive</t>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>FP</t>
+  </si>
+  <si>
+    <t>FN</t>
+  </si>
+  <si>
+    <t>TN</t>
   </si>
   <si>
     <t>Z Value</t>
   </si>
   <si>
-    <t>Critical Value (Channel G)</t>
-  </si>
-  <si>
-    <t>Critical Value (Channel F)</t>
+    <t>Critical Value (G)</t>
+  </si>
+  <si>
+    <t>Critical Value (F)</t>
   </si>
 </sst>
 </file>
@@ -323,8 +329,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,9 +379,6 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'ROC Data'!$A$2:$A$13</c:f>
@@ -481,9 +484,6 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'ROC Data'!$D$2:$D$14</c:f>
@@ -648,7 +648,7 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -700,16 +700,13 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-          </c:marker>
           <c:xVal>
             <c:strRef>
               <c:f>'ROC Data'!$H$2:$H$20</c:f>
               <c:strCache>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>True Positive</c:v>
+                  <c:v>TP</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>11</c:v>
@@ -902,7 +899,7 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4439,13 +4436,10 @@
       <c r="E1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -4462,20 +4456,20 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>13</v>
+      <c r="J2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -4569,8 +4563,8 @@
       <c r="E6">
         <v>0.4210526315789473</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>78</v>
+      <c r="G6" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="H6">
         <v>100</v>
@@ -4593,7 +4587,7 @@
         <v>0.5263157894736842</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H7">
         <v>3</v>
@@ -4616,7 +4610,7 @@
         <v>0.6578947368421053</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H8">
         <v>2.9</v>

</xml_diff>